<commit_message>
Currently writing functions on the fly and working on Vignettes/how to integrate a platemap. Now need to wrap up looping through the generated platemap.
Finished validating plates with multiple viruses.

Some QoLc changes on generate_platemap including prefilling with default values e.g. starting-dilution=2, dilution-series=1 in 3. TODO: allow user to define these prefill values.
</commit_message>
<xml_diff>
--- a/Validation/Example_PlateMap.xlsx
+++ b/Validation/Example_PlateMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\Dropbox (Cambridge University)\NormaliseForIC50\Validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02101614-2761-44FE-8EE6-169A27C56420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B91392F-AD02-4EAD-94BE-608DAD2BCE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4365" yWindow="1425" windowWidth="23055" windowHeight="13590" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4590" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7570B7-E159-4330-A885-FCB70407D2F9}">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I21"/>
+    <sheetView tabSelected="1" topLeftCell="D17" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1014,7 @@
         <v>13</v>
       </c>
       <c r="J12" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>14</v>
@@ -1049,7 +1049,7 @@
         <v>13</v>
       </c>
       <c r="J13" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>14</v>
@@ -1084,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="J14" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K14" s="8" t="s">
         <v>14</v>
@@ -1119,7 +1119,7 @@
         <v>13</v>
       </c>
       <c r="J15" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K15" s="8" t="s">
         <v>14</v>
@@ -1154,7 +1154,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K16" s="8" t="s">
         <v>14</v>
@@ -1189,7 +1189,7 @@
         <v>13</v>
       </c>
       <c r="J17" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>14</v>
@@ -1224,7 +1224,7 @@
         <v>13</v>
       </c>
       <c r="J18" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>14</v>
@@ -1259,7 +1259,7 @@
         <v>13</v>
       </c>
       <c r="J19" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>14</v>
@@ -1294,7 +1294,7 @@
         <v>13</v>
       </c>
       <c r="J20" s="8">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>14</v>
@@ -1328,8 +1328,8 @@
       <c r="I21" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="9">
-        <v>20</v>
+      <c r="J21" s="8">
+        <v>10</v>
       </c>
       <c r="K21" s="9" t="s">
         <v>14</v>
@@ -1345,7 +1345,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="A1:K25"/>
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,7 +2246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E334F8A7-C4B3-4267-844C-B4B9AEAE397B}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>